<commit_message>
added single vs multi
</commit_message>
<xml_diff>
--- a/Data/Permit_adjusted.xlsx
+++ b/Data/Permit_adjusted.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Google Sorenson Drive/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taohe/Documents/GitHub/SLC-Housing-Dashboard/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="980" windowWidth="28160" windowHeight="15420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="State Total" sheetId="2" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
-  <si>
-    <t>Year of Date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>Month of Date</t>
   </si>
@@ -262,6 +259,15 @@
   </si>
   <si>
     <t>Apartments/ 3 or 4 Family bldgs</t>
+  </si>
+  <si>
+    <t>2017 single vs multi</t>
+  </si>
+  <si>
+    <t>2017  single vs multi</t>
+  </si>
+  <si>
+    <t>Year of Date</t>
   </si>
 </sst>
 </file>
@@ -587,21 +593,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN82"/>
+  <dimension ref="A1:BN91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
     <col min="10" max="11" width="8.83203125" style="1"/>
     <col min="12" max="12" width="11.5" style="1" customWidth="1"/>
@@ -632,202 +636,202 @@
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BN1" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.2">
@@ -835,7 +839,7 @@
         <v>2011</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>228</v>
@@ -1035,7 +1039,7 @@
         <v>2011</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>228</v>
@@ -1235,7 +1239,7 @@
         <v>2011</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>228</v>
@@ -1435,7 +1439,7 @@
         <v>2011</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>228</v>
@@ -1635,7 +1639,7 @@
         <v>2011</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>228</v>
@@ -1835,7 +1839,7 @@
         <v>2011</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>228</v>
@@ -2035,7 +2039,7 @@
         <v>2011</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <v>228</v>
@@ -2235,7 +2239,7 @@
         <v>2011</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>228</v>
@@ -2435,7 +2439,7 @@
         <v>2011</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>228</v>
@@ -2635,7 +2639,7 @@
         <v>2011</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>228</v>
@@ -2835,7 +2839,7 @@
         <v>2011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>228</v>
@@ -3035,7 +3039,7 @@
         <v>2011</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <v>228</v>
@@ -3235,7 +3239,7 @@
         <v>2012</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
         <v>228</v>
@@ -3435,7 +3439,7 @@
         <v>2012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
         <v>228</v>
@@ -3635,7 +3639,7 @@
         <v>2012</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>228</v>
@@ -3835,7 +3839,7 @@
         <v>2012</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>228</v>
@@ -4035,7 +4039,7 @@
         <v>2012</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1">
         <v>228</v>
@@ -4235,7 +4239,7 @@
         <v>2012</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="1">
         <v>228</v>
@@ -4435,7 +4439,7 @@
         <v>2012</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="1">
         <v>228</v>
@@ -4635,7 +4639,7 @@
         <v>2012</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <v>228</v>
@@ -4835,7 +4839,7 @@
         <v>2012</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1">
         <v>228</v>
@@ -5035,7 +5039,7 @@
         <v>2012</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1">
         <v>228</v>
@@ -5235,7 +5239,7 @@
         <v>2012</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
         <v>228</v>
@@ -5435,7 +5439,7 @@
         <v>2012</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
         <v>228</v>
@@ -5635,7 +5639,7 @@
         <v>2013</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1">
         <v>228</v>
@@ -5835,7 +5839,7 @@
         <v>2013</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1">
         <v>228</v>
@@ -6035,7 +6039,7 @@
         <v>2013</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1">
         <v>228</v>
@@ -6235,7 +6239,7 @@
         <v>2013</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>228</v>
@@ -6435,7 +6439,7 @@
         <v>2013</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1">
         <v>228</v>
@@ -6635,7 +6639,7 @@
         <v>2013</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1">
         <v>228</v>
@@ -6835,7 +6839,7 @@
         <v>2013</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" s="1">
         <v>228</v>
@@ -7035,7 +7039,7 @@
         <v>2013</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>228</v>
@@ -7235,7 +7239,7 @@
         <v>2013</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1">
         <v>228</v>
@@ -7435,7 +7439,7 @@
         <v>2013</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="1">
         <v>228</v>
@@ -7635,7 +7639,7 @@
         <v>2013</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1">
         <v>228</v>
@@ -7835,7 +7839,7 @@
         <v>2013</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" s="1">
         <v>228</v>
@@ -8035,7 +8039,7 @@
         <v>2014</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
         <v>228</v>
@@ -8235,7 +8239,7 @@
         <v>2014</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
         <v>228</v>
@@ -8435,7 +8439,7 @@
         <v>2014</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1">
         <v>228</v>
@@ -8635,7 +8639,7 @@
         <v>2014</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1">
         <v>228</v>
@@ -8835,7 +8839,7 @@
         <v>2014</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1">
         <v>228</v>
@@ -9035,7 +9039,7 @@
         <v>2014</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1">
         <v>228</v>
@@ -9235,7 +9239,7 @@
         <v>2014</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C44" s="1">
         <v>228</v>
@@ -9435,7 +9439,7 @@
         <v>2014</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1">
         <v>228</v>
@@ -9635,7 +9639,7 @@
         <v>2014</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C46" s="1">
         <v>228</v>
@@ -9835,7 +9839,7 @@
         <v>2014</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="1">
         <v>228</v>
@@ -10035,7 +10039,7 @@
         <v>2014</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1">
         <v>228</v>
@@ -10235,7 +10239,7 @@
         <v>2014</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C49" s="1">
         <v>228</v>
@@ -10435,7 +10439,7 @@
         <v>2015</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1">
         <v>228</v>
@@ -10635,7 +10639,7 @@
         <v>2015</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1">
         <v>228</v>
@@ -10835,7 +10839,7 @@
         <v>2015</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C52" s="1">
         <v>228</v>
@@ -11035,7 +11039,7 @@
         <v>2015</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" s="1">
         <v>228</v>
@@ -11235,7 +11239,7 @@
         <v>2015</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1">
         <v>228</v>
@@ -11435,7 +11439,7 @@
         <v>2015</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1">
         <v>228</v>
@@ -11635,7 +11639,7 @@
         <v>2015</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56" s="1">
         <v>228</v>
@@ -11835,7 +11839,7 @@
         <v>2015</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C57" s="1">
         <v>228</v>
@@ -12035,7 +12039,7 @@
         <v>2015</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58" s="1">
         <v>228</v>
@@ -12235,7 +12239,7 @@
         <v>2015</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" s="1">
         <v>228</v>
@@ -12435,7 +12439,7 @@
         <v>2015</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C60" s="1">
         <v>228</v>
@@ -12635,7 +12639,7 @@
         <v>2015</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C61" s="1">
         <v>228</v>
@@ -12835,7 +12839,7 @@
         <v>2016</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62" s="1">
         <v>229</v>
@@ -13035,7 +13039,7 @@
         <v>2016</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1">
         <v>229</v>
@@ -13235,7 +13239,7 @@
         <v>2016</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1">
         <v>229</v>
@@ -13435,7 +13439,7 @@
         <v>2016</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1">
         <v>229</v>
@@ -13635,7 +13639,7 @@
         <v>2016</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C66" s="1">
         <v>229</v>
@@ -13835,7 +13839,7 @@
         <v>2016</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" s="1">
         <v>229</v>
@@ -14035,7 +14039,7 @@
         <v>2016</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C68" s="1">
         <v>229</v>
@@ -14235,7 +14239,7 @@
         <v>2016</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1">
         <v>229</v>
@@ -14435,7 +14439,7 @@
         <v>2016</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C70" s="1">
         <v>229</v>
@@ -14635,7 +14639,7 @@
         <v>2016</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71" s="1">
         <v>229</v>
@@ -14835,7 +14839,7 @@
         <v>2016</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C72" s="1">
         <v>229</v>
@@ -15035,7 +15039,7 @@
         <v>2016</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C73" s="1">
         <v>229</v>
@@ -15235,7 +15239,7 @@
         <v>2017</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1">
         <v>229</v>
@@ -15435,7 +15439,7 @@
         <v>2017</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75" s="1">
         <v>229</v>
@@ -15635,7 +15639,7 @@
         <v>2017</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1">
         <v>229</v>
@@ -15835,7 +15839,7 @@
         <v>2017</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" s="1">
         <v>229</v>
@@ -16035,7 +16039,7 @@
         <v>2017</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1">
         <v>229</v>
@@ -16235,7 +16239,7 @@
         <v>2017</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" s="1">
         <v>229</v>
@@ -16435,7 +16439,7 @@
         <v>2017</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C80" s="1">
         <v>229</v>
@@ -16635,7 +16639,7 @@
         <v>2017</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C81" s="1">
         <v>229</v>
@@ -16835,7 +16839,7 @@
         <v>2017</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C82" s="1">
         <v>229</v>
@@ -17028,10 +17032,156 @@
       </c>
       <c r="BN82" s="2">
         <v>73414518</v>
+      </c>
+    </row>
+    <row r="83" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="1">
+        <f t="shared" ref="E83:E91" si="0">E74</f>
+        <v>611</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" ref="H83:H91" si="1">H74+K74+N74+Q74</f>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="84" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="0"/>
+        <v>778</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="1"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="85" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="2">
+        <f t="shared" si="0"/>
+        <v>1055</v>
+      </c>
+      <c r="H85" s="2">
+        <f t="shared" si="1"/>
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="86" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="0"/>
+        <v>992</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="1"/>
+        <v>884</v>
+      </c>
+    </row>
+    <row r="87" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="2">
+        <f t="shared" si="0"/>
+        <v>1181</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="1"/>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="88" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="2">
+        <f t="shared" si="0"/>
+        <v>1359</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="1"/>
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="89" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="2">
+        <f t="shared" si="0"/>
+        <v>1061</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="1"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="90" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="2">
+        <f t="shared" si="0"/>
+        <v>1281</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="1"/>
+        <v>872</v>
+      </c>
+    </row>
+    <row r="91" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E91" s="2">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="1"/>
+        <v>1021</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>